<commit_message>
increased timeout limit, added cat feedback, switched to data.table
</commit_message>
<xml_diff>
--- a/output/parameters_in_database.xlsx
+++ b/output/parameters_in_database.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="271">
   <si>
     <t xml:space="preserve">PARAMETER</t>
   </si>
@@ -26,28 +26,49 @@
     <t xml:space="preserve">Phosphorus Total</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-07-24 - 2024-08-02</t>
+    <t xml:space="preserve">2024-08-02 - 2024-08-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phosphorus Total Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrate (NO3) Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH</t>
   </si>
   <si>
     <t xml:space="preserve">Residue: Non-filterable (TSS)</t>
   </si>
   <si>
-    <t xml:space="preserve">Phosphorus Total Dissolved</t>
+    <t xml:space="preserve">Sulfate Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrate(NO3) + Nitrite(NO2) Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen - Nitrite Dissolved (NO2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hardness (Dissolved) (as CaCO3)</t>
   </si>
   <si>
     <t xml:space="preserve">Turbidity</t>
   </si>
   <si>
-    <t xml:space="preserve">Sulfate Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrate (NO3) Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hardness (Dissolved) (as CaCO3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH</t>
+    <t xml:space="preserve">Specific Conductance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chloride Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen Ammonia Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hardness Total (Total)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selenium Total</t>
   </si>
   <si>
     <t xml:space="preserve">Calcium Dissolved</t>
@@ -56,433 +77,754 @@
     <t xml:space="preserve">Magnesium Dissolved</t>
   </si>
   <si>
-    <t xml:space="preserve">Nitrate(NO3) + Nitrite(NO2) Dissolved</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sodium Dissolved</t>
   </si>
   <si>
     <t xml:space="preserve">Potassium Dissolved</t>
   </si>
   <si>
+    <t xml:space="preserve">Calcium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnesium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phosphorus Ort.Dis-P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copper Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sodium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluminum Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadmium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manganese Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molybdenum Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zinc Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antimony Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arsenic Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boron Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadmium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cobalt Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copper Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nickel Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selenium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strontium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uranium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluminum Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antimony Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arsenic Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beryllium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bismuth Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boron Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chromium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cobalt Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lead Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manganese Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molybdenum Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nickel Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potassium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicon Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicon Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strontium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thallium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tin Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uranium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanadium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zinc Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beryllium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bismuth Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chromium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lead Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thallium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tin Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanadium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lithium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lithium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titanium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alkalinity Total 4.5 (as CaCO3)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Carbon Dissolved Organic</t>
   </si>
   <si>
-    <t xml:space="preserve">Hardness Total (Total)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selenium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen - Nitrite Dissolved (NO2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chloride Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copper Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manganese Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Molybdenum Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zinc Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aluminum Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antimony Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arsenic Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beryllium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bismuth Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boron Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cadmium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chromium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cobalt Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lead Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nickel Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selenium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silicon Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silver Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strontium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thallium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tin Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uranium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanadium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alkalinity Total 4.5 (as CaCO3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aluminum Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antimony Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arsenic Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beryllium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bismuth Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boron Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cadmium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chromium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cobalt Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copper Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lead Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magnesium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manganese Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Molybdenum Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nickel Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potassium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silicon Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silver Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sodium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strontium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thallium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tin Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uranium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanadium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zinc Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specific Conductance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lithium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen Ammonia Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Titanium Dissolved</t>
+    <t xml:space="preserve">Titanium Total</t>
   </si>
   <si>
     <t xml:space="preserve">Sulfur Dissolved</t>
   </si>
   <si>
-    <t xml:space="preserve">Lithium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Titanium Total</t>
+    <t xml:space="preserve">Residue: Filterable 1.0u (TDS)</t>
   </si>
   <si>
     <t xml:space="preserve">Sulfur Total</t>
   </si>
   <si>
-    <t xml:space="preserve">Phosphorus Ort.Dis-P</t>
-  </si>
-  <si>
     <t xml:space="preserve">Zirconium Dissolved</t>
   </si>
   <si>
-    <t xml:space="preserve">Residue: Filterable 1.0u (TDS)</t>
+    <t xml:space="preserve">Fluoride Dissolved</t>
   </si>
   <si>
     <t xml:space="preserve">Residue: Total (Total Solids)</t>
   </si>
   <si>
+    <t xml:space="preserve">Nitrogen Kjel.Tot(N)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zirconium Total</t>
   </si>
   <si>
+    <t xml:space="preserve">Bromide Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon Total Organic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen Organic-Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Nitrogen NO2 + NO3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tellerium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thorium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tungsten Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tellurium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thorium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tungsten Total</t>
+  </si>
+  <si>
     <t xml:space="preserve">Temperature-Field</t>
   </si>
   <si>
-    <t xml:space="preserve">Fluoride Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen Kjel.Tot(N)</t>
+    <t xml:space="preserve">Mercury Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bicarbonate Alkalinity (as CaCO3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbonate Alkalinity (as CaCO3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydroxide Alkalinity (as CaCO3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mercury Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cesium Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rubidium Dissolved</t>
   </si>
   <si>
     <t xml:space="preserve">Dissolved Oxygen-Field</t>
   </si>
   <si>
-    <t xml:space="preserve">Tellurium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thorium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tungsten Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mercury Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mercury Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tellerium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thorium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tungsten Dissolved</t>
+    <t xml:space="preserve">Color True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific Conductivity-Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH-Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cesium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rubidium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alkalinity; Phenolphthalein (as CaCO3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acidity pH 8.3 (as CaCO3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen Ammonia Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorophyll A</t>
   </si>
   <si>
     <t xml:space="preserve">E Coli</t>
   </si>
   <si>
-    <t xml:space="preserve">Specific Conductivity-Field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bromide Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Nitrogen NO2 + NO3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bicarbonate Alkalinity (as CaCO3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carbon Total Organic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carbonate Alkalinity (as CaCO3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hydroxide Alkalinity (as CaCO3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alkalinity; Phenolphthalein (as CaCO3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cesium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen Organic-Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rubidium Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cesium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rubidium Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH-Field</t>
-  </si>
-  <si>
     <t xml:space="preserve">Biochemical Oxygen Demand</t>
   </si>
   <si>
-    <t xml:space="preserve">Color True</t>
+    <t xml:space="preserve">Cyanide Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyanide WAD</t>
   </si>
   <si>
     <t xml:space="preserve">Oxid. Red. Potential</t>
   </si>
   <si>
+    <t xml:space="preserve">Thiocyanate Dissolved</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coliform - Fecal</t>
   </si>
   <si>
-    <t xml:space="preserve">Nitrogen Ammonia Dissolved</t>
+    <t xml:space="preserve">Sulfide Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydrogen Sulfide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cation-Anion Balance %=100*(Cations-Anions)/(Cations+Anions)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silica Reactive Diss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical Oxygen Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anion Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cation Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extinction Depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen Total Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chromium; Hexavalent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluoride Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chromium; Hexavalent; Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen (Kjeldahl) Total Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxid. Red. Potential- Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbonaceous Biochemical Oxygen Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown Selenium Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenate SeO4(-2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenite SeO3(-2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenocyanate SeCN(-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acidity pH 4.5 (as CaCO3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorine Res:Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen, dissolved saturation %, field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turbidity-Field	</t>
   </si>
   <si>
     <t xml:space="preserve">Flow (Avg)</t>
   </si>
   <si>
-    <t xml:space="preserve">Hydrogen Sulfide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acidity pH 8.3 (as CaCO3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical Oxygen Demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sulfide Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chlorophyll A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acidity pH 4.5 (as CaCO3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyanide Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyanide WAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turbidity-Field	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen Total Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen, dissolved saturation %, field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen (Kjeldahl) Total Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thiocyanate Dissolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluoride Total</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nitrogen Organic Total Dissolved</t>
   </si>
   <si>
-    <t xml:space="preserve">Carbonaceous Biochemical Oxygen Demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extinction Depth</t>
+    <t xml:space="preserve">Un-ionized Ammonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bromobenzotrifluoride, 2 (EPH surr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimethyl Diselenide [DMDSe]; as Se</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimethyl Selenide [DMSe]; as Se</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unidentified Volatile Selenium Species (As Se)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">methylseleninic acid CH3SeO2H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenomethionine CH3SeCH2CH2CH(NH2)CO2H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heavy Extractable Petroleum Hydrocarbons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HydroC Extrct/C10-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light Extractable Petroleum Hydrocarbons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coliform - Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oil &amp; Grease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gallium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lathanum Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niobium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhenium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tantalum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yttrium Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bicarbonate (CAS 71-52-3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carbonate (CAS 3812-32-6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hydroxide (CAS 14280-30-9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;4-Difluorobenzene (IS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-Bromofluorobenzene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benzene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chromium; Trivalent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterococcus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethylbenzene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M;P-Xylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radium-226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Styrene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toluene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o-Xylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon Dissolved Inorganic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon Total Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyanate Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrical Conductivity - Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydrocarbons; Volatile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydrocarbons; Volatile Petroleum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Met.Tert.Butyl Ether</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salinity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surrogate standard used for VH analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Methylnaphthalene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Methylnaphthalene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acenaphthene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acenaphthylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acridine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anthracene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benzo(a)anthracene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benzo(a)pyrene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benzo(b+j)fluoranthene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benzo(b;j;k)fluoranthene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benzo(g;h;i)perylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benzo(k)fluoranthene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chromium; Trivalent; Dissolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chrysene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chrysene d12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dibenzo(a;h)anthracene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluoranthene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluorene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indeno(1;2;3-cd)pyrene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naphthalene (C10H8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naphthalene d8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oil&amp;Grease (Mineral)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phenanthrene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phenanthrene d10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyrene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quinoline aka Benzo(b)pyridine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Solids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;1-Dichloroethane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;1-Dichloroethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;1;1-Trichloroethane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;1;1;2-Tetrachloroethane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;1;2-Trichloroethane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;1;2;2-Tetrachloroethane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;2 Dichlorobenzene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;2-Dichloroethane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;2-Dichloropropane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;3-Dichlorobenzene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;3-Dichloropropene (cis &amp; trans)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1;4-Dichlorobenzene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4,6-Tribromophenol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4-Dichlorophenol-d3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Chlorophenol-d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alkalinity:Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bromodichloromethane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bromoform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon Tetrachloride</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon Total Inorganic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorine, total, field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorobenzene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorodibromomethane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chloroethane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chloroform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chloromethane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dichloromethane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimethylphenol-2;4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heterotrophic Plate Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen Dioxide</t>
   </si>
   <si>
     <t xml:space="preserve">Nitrogen Total Inorganic</t>
   </si>
   <si>
-    <t xml:space="preserve">Enterococcus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxid. Red. Potential- Field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silica Reactive Diss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UV Absorbance 254nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un-ionized Ammonia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anion Sum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cation Sum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cation-Anion Balance %=100*(Cations-Anions)/(Cations+Anions)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chlorine Dioxide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chlorine Res:Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coliform - Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residue: Fixed Non-filterable (TSS; Fixed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residue: Volatile Non-filterable (TSS; Volatile)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surfactants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume Flow Rate-Stk</t>
+    <t xml:space="preserve">Particulate &lt;10u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Particulate &lt;2.5u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phenol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phenols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sulfur Dioxide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tetrachloroethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total coarse particulates in air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total fine particulates in air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trichloroethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trichlorofluoromethane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinyl Chloride</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cis-1;2-DiClethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cis-1;3-Dichloropropene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m-Cresol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o-Cresol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p-Cresol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trans1;2-Dichloroethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trans1;3-Dichloropropene</t>
   </si>
 </sst>
 </file>
@@ -830,7 +1172,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>169</v>
+        <v>756</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -841,7 +1183,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>158</v>
+        <v>654</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -852,7 +1194,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>157</v>
+        <v>544</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -863,7 +1205,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>127</v>
+        <v>517</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -874,7 +1216,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>122</v>
+        <v>505</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -885,7 +1227,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>114</v>
+        <v>495</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -896,7 +1238,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>113</v>
+        <v>493</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -907,7 +1249,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>107</v>
+        <v>488</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -918,7 +1260,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>106</v>
+        <v>474</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -929,7 +1271,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>106</v>
+        <v>466</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -940,7 +1282,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -951,7 +1293,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>100</v>
+        <v>444</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -962,7 +1304,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>98</v>
+        <v>428</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -973,7 +1315,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>97</v>
+        <v>422</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -984,7 +1326,7 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>94</v>
+        <v>421</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -995,7 +1337,7 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>94</v>
+        <v>420</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -1006,7 +1348,7 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>93</v>
+        <v>420</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1017,7 +1359,7 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>93</v>
+        <v>415</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -1028,7 +1370,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>92</v>
+        <v>414</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -1039,7 +1381,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>92</v>
+        <v>402</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -1050,7 +1392,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>92</v>
+        <v>402</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -1061,7 +1403,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>92</v>
+        <v>395</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -1072,7 +1414,7 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>92</v>
+        <v>393</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -1083,7 +1425,7 @@
         <v>27</v>
       </c>
       <c r="B25" t="n">
-        <v>91</v>
+        <v>393</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1094,7 +1436,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="n">
-        <v>90</v>
+        <v>391</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -1105,7 +1447,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="n">
-        <v>90</v>
+        <v>391</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1116,7 +1458,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="n">
-        <v>90</v>
+        <v>391</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -1127,7 +1469,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="n">
-        <v>90</v>
+        <v>391</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -1138,7 +1480,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="n">
-        <v>90</v>
+        <v>391</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -1149,7 +1491,7 @@
         <v>33</v>
       </c>
       <c r="B31" t="n">
-        <v>90</v>
+        <v>391</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -1160,7 +1502,7 @@
         <v>34</v>
       </c>
       <c r="B32" t="n">
-        <v>90</v>
+        <v>390</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -1171,7 +1513,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="n">
-        <v>90</v>
+        <v>390</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -1182,7 +1524,7 @@
         <v>36</v>
       </c>
       <c r="B34" t="n">
-        <v>90</v>
+        <v>390</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -1193,7 +1535,7 @@
         <v>37</v>
       </c>
       <c r="B35" t="n">
-        <v>90</v>
+        <v>390</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -1204,7 +1546,7 @@
         <v>38</v>
       </c>
       <c r="B36" t="n">
-        <v>90</v>
+        <v>390</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -1215,7 +1557,7 @@
         <v>39</v>
       </c>
       <c r="B37" t="n">
-        <v>90</v>
+        <v>390</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -1226,7 +1568,7 @@
         <v>40</v>
       </c>
       <c r="B38" t="n">
-        <v>90</v>
+        <v>390</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -1237,7 +1579,7 @@
         <v>41</v>
       </c>
       <c r="B39" t="n">
-        <v>90</v>
+        <v>390</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
@@ -1248,7 +1590,7 @@
         <v>42</v>
       </c>
       <c r="B40" t="n">
-        <v>90</v>
+        <v>390</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -1259,7 +1601,7 @@
         <v>43</v>
       </c>
       <c r="B41" t="n">
-        <v>90</v>
+        <v>390</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -1270,7 +1612,7 @@
         <v>44</v>
       </c>
       <c r="B42" t="n">
-        <v>90</v>
+        <v>390</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
@@ -1281,7 +1623,7 @@
         <v>45</v>
       </c>
       <c r="B43" t="n">
-        <v>90</v>
+        <v>390</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
@@ -1292,7 +1634,7 @@
         <v>46</v>
       </c>
       <c r="B44" t="n">
-        <v>90</v>
+        <v>389</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
@@ -1303,7 +1645,7 @@
         <v>47</v>
       </c>
       <c r="B45" t="n">
-        <v>90</v>
+        <v>389</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
@@ -1314,7 +1656,7 @@
         <v>48</v>
       </c>
       <c r="B46" t="n">
-        <v>86</v>
+        <v>389</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
@@ -1325,7 +1667,7 @@
         <v>49</v>
       </c>
       <c r="B47" t="n">
-        <v>85</v>
+        <v>389</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -1336,7 +1678,7 @@
         <v>50</v>
       </c>
       <c r="B48" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
@@ -1347,7 +1689,7 @@
         <v>51</v>
       </c>
       <c r="B49" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C49" t="s">
         <v>4</v>
@@ -1358,7 +1700,7 @@
         <v>52</v>
       </c>
       <c r="B50" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
@@ -1369,7 +1711,7 @@
         <v>53</v>
       </c>
       <c r="B51" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
@@ -1380,7 +1722,7 @@
         <v>54</v>
       </c>
       <c r="B52" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C52" t="s">
         <v>4</v>
@@ -1391,7 +1733,7 @@
         <v>55</v>
       </c>
       <c r="B53" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C53" t="s">
         <v>4</v>
@@ -1402,7 +1744,7 @@
         <v>56</v>
       </c>
       <c r="B54" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C54" t="s">
         <v>4</v>
@@ -1413,7 +1755,7 @@
         <v>57</v>
       </c>
       <c r="B55" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C55" t="s">
         <v>4</v>
@@ -1424,7 +1766,7 @@
         <v>58</v>
       </c>
       <c r="B56" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C56" t="s">
         <v>4</v>
@@ -1435,7 +1777,7 @@
         <v>59</v>
       </c>
       <c r="B57" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C57" t="s">
         <v>4</v>
@@ -1446,7 +1788,7 @@
         <v>60</v>
       </c>
       <c r="B58" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C58" t="s">
         <v>4</v>
@@ -1457,7 +1799,7 @@
         <v>61</v>
       </c>
       <c r="B59" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C59" t="s">
         <v>4</v>
@@ -1468,7 +1810,7 @@
         <v>62</v>
       </c>
       <c r="B60" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
@@ -1479,7 +1821,7 @@
         <v>63</v>
       </c>
       <c r="B61" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
@@ -1490,7 +1832,7 @@
         <v>64</v>
       </c>
       <c r="B62" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
@@ -1501,7 +1843,7 @@
         <v>65</v>
       </c>
       <c r="B63" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C63" t="s">
         <v>4</v>
@@ -1512,7 +1854,7 @@
         <v>66</v>
       </c>
       <c r="B64" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C64" t="s">
         <v>4</v>
@@ -1523,7 +1865,7 @@
         <v>67</v>
       </c>
       <c r="B65" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C65" t="s">
         <v>4</v>
@@ -1534,7 +1876,7 @@
         <v>68</v>
       </c>
       <c r="B66" t="n">
-        <v>84</v>
+        <v>389</v>
       </c>
       <c r="C66" t="s">
         <v>4</v>
@@ -1545,7 +1887,7 @@
         <v>69</v>
       </c>
       <c r="B67" t="n">
-        <v>84</v>
+        <v>388</v>
       </c>
       <c r="C67" t="s">
         <v>4</v>
@@ -1556,7 +1898,7 @@
         <v>70</v>
       </c>
       <c r="B68" t="n">
-        <v>84</v>
+        <v>388</v>
       </c>
       <c r="C68" t="s">
         <v>4</v>
@@ -1567,7 +1909,7 @@
         <v>71</v>
       </c>
       <c r="B69" t="n">
-        <v>84</v>
+        <v>388</v>
       </c>
       <c r="C69" t="s">
         <v>4</v>
@@ -1578,7 +1920,7 @@
         <v>72</v>
       </c>
       <c r="B70" t="n">
-        <v>84</v>
+        <v>388</v>
       </c>
       <c r="C70" t="s">
         <v>4</v>
@@ -1589,7 +1931,7 @@
         <v>73</v>
       </c>
       <c r="B71" t="n">
-        <v>84</v>
+        <v>388</v>
       </c>
       <c r="C71" t="s">
         <v>4</v>
@@ -1600,7 +1942,7 @@
         <v>74</v>
       </c>
       <c r="B72" t="n">
-        <v>84</v>
+        <v>388</v>
       </c>
       <c r="C72" t="s">
         <v>4</v>
@@ -1611,7 +1953,7 @@
         <v>75</v>
       </c>
       <c r="B73" t="n">
-        <v>84</v>
+        <v>388</v>
       </c>
       <c r="C73" t="s">
         <v>4</v>
@@ -1622,7 +1964,7 @@
         <v>76</v>
       </c>
       <c r="B74" t="n">
-        <v>84</v>
+        <v>388</v>
       </c>
       <c r="C74" t="s">
         <v>4</v>
@@ -1633,7 +1975,7 @@
         <v>77</v>
       </c>
       <c r="B75" t="n">
-        <v>83</v>
+        <v>377</v>
       </c>
       <c r="C75" t="s">
         <v>4</v>
@@ -1644,7 +1986,7 @@
         <v>78</v>
       </c>
       <c r="B76" t="n">
-        <v>82</v>
+        <v>371</v>
       </c>
       <c r="C76" t="s">
         <v>4</v>
@@ -1655,7 +1997,7 @@
         <v>79</v>
       </c>
       <c r="B77" t="n">
-        <v>81</v>
+        <v>370</v>
       </c>
       <c r="C77" t="s">
         <v>4</v>
@@ -1666,7 +2008,7 @@
         <v>80</v>
       </c>
       <c r="B78" t="n">
-        <v>81</v>
+        <v>369</v>
       </c>
       <c r="C78" t="s">
         <v>4</v>
@@ -1677,7 +2019,7 @@
         <v>81</v>
       </c>
       <c r="B79" t="n">
-        <v>79</v>
+        <v>368</v>
       </c>
       <c r="C79" t="s">
         <v>4</v>
@@ -1688,7 +2030,7 @@
         <v>82</v>
       </c>
       <c r="B80" t="n">
-        <v>76</v>
+        <v>367</v>
       </c>
       <c r="C80" t="s">
         <v>4</v>
@@ -1699,7 +2041,7 @@
         <v>83</v>
       </c>
       <c r="B81" t="n">
-        <v>75</v>
+        <v>338</v>
       </c>
       <c r="C81" t="s">
         <v>4</v>
@@ -1710,7 +2052,7 @@
         <v>84</v>
       </c>
       <c r="B82" t="n">
-        <v>74</v>
+        <v>326</v>
       </c>
       <c r="C82" t="s">
         <v>4</v>
@@ -1721,7 +2063,7 @@
         <v>85</v>
       </c>
       <c r="B83" t="n">
-        <v>72</v>
+        <v>318</v>
       </c>
       <c r="C83" t="s">
         <v>4</v>
@@ -1732,7 +2074,7 @@
         <v>86</v>
       </c>
       <c r="B84" t="n">
-        <v>67</v>
+        <v>301</v>
       </c>
       <c r="C84" t="s">
         <v>4</v>
@@ -1743,7 +2085,7 @@
         <v>87</v>
       </c>
       <c r="B85" t="n">
-        <v>65</v>
+        <v>286</v>
       </c>
       <c r="C85" t="s">
         <v>4</v>
@@ -1754,7 +2096,7 @@
         <v>88</v>
       </c>
       <c r="B86" t="n">
-        <v>64</v>
+        <v>283</v>
       </c>
       <c r="C86" t="s">
         <v>4</v>
@@ -1765,7 +2107,7 @@
         <v>89</v>
       </c>
       <c r="B87" t="n">
-        <v>64</v>
+        <v>278</v>
       </c>
       <c r="C87" t="s">
         <v>4</v>
@@ -1776,7 +2118,7 @@
         <v>90</v>
       </c>
       <c r="B88" t="n">
-        <v>52</v>
+        <v>269</v>
       </c>
       <c r="C88" t="s">
         <v>4</v>
@@ -1787,7 +2129,7 @@
         <v>91</v>
       </c>
       <c r="B89" t="n">
-        <v>51</v>
+        <v>262</v>
       </c>
       <c r="C89" t="s">
         <v>4</v>
@@ -1798,7 +2140,7 @@
         <v>92</v>
       </c>
       <c r="B90" t="n">
-        <v>48</v>
+        <v>241</v>
       </c>
       <c r="C90" t="s">
         <v>4</v>
@@ -1809,7 +2151,7 @@
         <v>93</v>
       </c>
       <c r="B91" t="n">
-        <v>47</v>
+        <v>221</v>
       </c>
       <c r="C91" t="s">
         <v>4</v>
@@ -1820,7 +2162,7 @@
         <v>94</v>
       </c>
       <c r="B92" t="n">
-        <v>43</v>
+        <v>214</v>
       </c>
       <c r="C92" t="s">
         <v>4</v>
@@ -1831,7 +2173,7 @@
         <v>95</v>
       </c>
       <c r="B93" t="n">
-        <v>43</v>
+        <v>212</v>
       </c>
       <c r="C93" t="s">
         <v>4</v>
@@ -1842,7 +2184,7 @@
         <v>96</v>
       </c>
       <c r="B94" t="n">
-        <v>43</v>
+        <v>208</v>
       </c>
       <c r="C94" t="s">
         <v>4</v>
@@ -1853,7 +2195,7 @@
         <v>97</v>
       </c>
       <c r="B95" t="n">
-        <v>42</v>
+        <v>208</v>
       </c>
       <c r="C95" t="s">
         <v>4</v>
@@ -1864,7 +2206,7 @@
         <v>98</v>
       </c>
       <c r="B96" t="n">
-        <v>42</v>
+        <v>208</v>
       </c>
       <c r="C96" t="s">
         <v>4</v>
@@ -1875,7 +2217,7 @@
         <v>99</v>
       </c>
       <c r="B97" t="n">
-        <v>42</v>
+        <v>192</v>
       </c>
       <c r="C97" t="s">
         <v>4</v>
@@ -1886,7 +2228,7 @@
         <v>100</v>
       </c>
       <c r="B98" t="n">
-        <v>42</v>
+        <v>192</v>
       </c>
       <c r="C98" t="s">
         <v>4</v>
@@ -1897,7 +2239,7 @@
         <v>101</v>
       </c>
       <c r="B99" t="n">
-        <v>42</v>
+        <v>192</v>
       </c>
       <c r="C99" t="s">
         <v>4</v>
@@ -1908,7 +2250,7 @@
         <v>102</v>
       </c>
       <c r="B100" t="n">
-        <v>41</v>
+        <v>186</v>
       </c>
       <c r="C100" t="s">
         <v>4</v>
@@ -1919,7 +2261,7 @@
         <v>103</v>
       </c>
       <c r="B101" t="n">
-        <v>41</v>
+        <v>181</v>
       </c>
       <c r="C101" t="s">
         <v>4</v>
@@ -1930,7 +2272,7 @@
         <v>104</v>
       </c>
       <c r="B102" t="n">
-        <v>40</v>
+        <v>172</v>
       </c>
       <c r="C102" t="s">
         <v>4</v>
@@ -1941,7 +2283,7 @@
         <v>105</v>
       </c>
       <c r="B103" t="n">
-        <v>40</v>
+        <v>172</v>
       </c>
       <c r="C103" t="s">
         <v>4</v>
@@ -1952,7 +2294,7 @@
         <v>106</v>
       </c>
       <c r="B104" t="n">
-        <v>39</v>
+        <v>172</v>
       </c>
       <c r="C104" t="s">
         <v>4</v>
@@ -1963,7 +2305,7 @@
         <v>107</v>
       </c>
       <c r="B105" t="n">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="C105" t="s">
         <v>4</v>
@@ -1974,7 +2316,7 @@
         <v>108</v>
       </c>
       <c r="B106" t="n">
-        <v>39</v>
+        <v>162</v>
       </c>
       <c r="C106" t="s">
         <v>4</v>
@@ -1985,7 +2327,7 @@
         <v>109</v>
       </c>
       <c r="B107" t="n">
-        <v>39</v>
+        <v>162</v>
       </c>
       <c r="C107" t="s">
         <v>4</v>
@@ -1996,7 +2338,7 @@
         <v>110</v>
       </c>
       <c r="B108" t="n">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="C108" t="s">
         <v>4</v>
@@ -2007,7 +2349,7 @@
         <v>111</v>
       </c>
       <c r="B109" t="n">
-        <v>36</v>
+        <v>146</v>
       </c>
       <c r="C109" t="s">
         <v>4</v>
@@ -2018,7 +2360,7 @@
         <v>112</v>
       </c>
       <c r="B110" t="n">
-        <v>36</v>
+        <v>146</v>
       </c>
       <c r="C110" t="s">
         <v>4</v>
@@ -2029,7 +2371,7 @@
         <v>113</v>
       </c>
       <c r="B111" t="n">
-        <v>36</v>
+        <v>143</v>
       </c>
       <c r="C111" t="s">
         <v>4</v>
@@ -2040,7 +2382,7 @@
         <v>114</v>
       </c>
       <c r="B112" t="n">
-        <v>35</v>
+        <v>138</v>
       </c>
       <c r="C112" t="s">
         <v>4</v>
@@ -2051,7 +2393,7 @@
         <v>115</v>
       </c>
       <c r="B113" t="n">
-        <v>35</v>
+        <v>138</v>
       </c>
       <c r="C113" t="s">
         <v>4</v>
@@ -2062,7 +2404,7 @@
         <v>116</v>
       </c>
       <c r="B114" t="n">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="C114" t="s">
         <v>4</v>
@@ -2073,7 +2415,7 @@
         <v>117</v>
       </c>
       <c r="B115" t="n">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="C115" t="s">
         <v>4</v>
@@ -2084,7 +2426,7 @@
         <v>118</v>
       </c>
       <c r="B116" t="n">
-        <v>24</v>
+        <v>97</v>
       </c>
       <c r="C116" t="s">
         <v>4</v>
@@ -2095,7 +2437,7 @@
         <v>119</v>
       </c>
       <c r="B117" t="n">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="C117" t="s">
         <v>4</v>
@@ -2106,7 +2448,7 @@
         <v>120</v>
       </c>
       <c r="B118" t="n">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="C118" t="s">
         <v>4</v>
@@ -2117,7 +2459,7 @@
         <v>121</v>
       </c>
       <c r="B119" t="n">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="C119" t="s">
         <v>4</v>
@@ -2128,7 +2470,7 @@
         <v>122</v>
       </c>
       <c r="B120" t="n">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="C120" t="s">
         <v>4</v>
@@ -2139,7 +2481,7 @@
         <v>123</v>
       </c>
       <c r="B121" t="n">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="C121" t="s">
         <v>4</v>
@@ -2150,7 +2492,7 @@
         <v>124</v>
       </c>
       <c r="B122" t="n">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="C122" t="s">
         <v>4</v>
@@ -2161,7 +2503,7 @@
         <v>125</v>
       </c>
       <c r="B123" t="n">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="C123" t="s">
         <v>4</v>
@@ -2172,7 +2514,7 @@
         <v>126</v>
       </c>
       <c r="B124" t="n">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="C124" t="s">
         <v>4</v>
@@ -2183,7 +2525,7 @@
         <v>127</v>
       </c>
       <c r="B125" t="n">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C125" t="s">
         <v>4</v>
@@ -2194,7 +2536,7 @@
         <v>128</v>
       </c>
       <c r="B126" t="n">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C126" t="s">
         <v>4</v>
@@ -2205,7 +2547,7 @@
         <v>129</v>
       </c>
       <c r="B127" t="n">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C127" t="s">
         <v>4</v>
@@ -2216,7 +2558,7 @@
         <v>130</v>
       </c>
       <c r="B128" t="n">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="C128" t="s">
         <v>4</v>
@@ -2227,7 +2569,7 @@
         <v>131</v>
       </c>
       <c r="B129" t="n">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C129" t="s">
         <v>4</v>
@@ -2238,7 +2580,7 @@
         <v>132</v>
       </c>
       <c r="B130" t="n">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C130" t="s">
         <v>4</v>
@@ -2249,7 +2591,7 @@
         <v>133</v>
       </c>
       <c r="B131" t="n">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C131" t="s">
         <v>4</v>
@@ -2260,7 +2602,7 @@
         <v>134</v>
       </c>
       <c r="B132" t="n">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C132" t="s">
         <v>4</v>
@@ -2271,7 +2613,7 @@
         <v>135</v>
       </c>
       <c r="B133" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C133" t="s">
         <v>4</v>
@@ -2282,7 +2624,7 @@
         <v>136</v>
       </c>
       <c r="B134" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C134" t="s">
         <v>4</v>
@@ -2293,7 +2635,7 @@
         <v>137</v>
       </c>
       <c r="B135" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C135" t="s">
         <v>4</v>
@@ -2304,7 +2646,7 @@
         <v>138</v>
       </c>
       <c r="B136" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C136" t="s">
         <v>4</v>
@@ -2315,7 +2657,7 @@
         <v>139</v>
       </c>
       <c r="B137" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C137" t="s">
         <v>4</v>
@@ -2326,7 +2668,7 @@
         <v>140</v>
       </c>
       <c r="B138" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C138" t="s">
         <v>4</v>
@@ -2337,7 +2679,7 @@
         <v>141</v>
       </c>
       <c r="B139" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C139" t="s">
         <v>4</v>
@@ -2348,7 +2690,7 @@
         <v>142</v>
       </c>
       <c r="B140" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C140" t="s">
         <v>4</v>
@@ -2359,7 +2701,7 @@
         <v>143</v>
       </c>
       <c r="B141" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C141" t="s">
         <v>4</v>
@@ -2370,7 +2712,7 @@
         <v>144</v>
       </c>
       <c r="B142" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C142" t="s">
         <v>4</v>
@@ -2381,7 +2723,7 @@
         <v>145</v>
       </c>
       <c r="B143" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C143" t="s">
         <v>4</v>
@@ -2392,7 +2734,7 @@
         <v>146</v>
       </c>
       <c r="B144" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C144" t="s">
         <v>4</v>
@@ -2403,7 +2745,7 @@
         <v>147</v>
       </c>
       <c r="B145" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C145" t="s">
         <v>4</v>
@@ -2414,7 +2756,7 @@
         <v>148</v>
       </c>
       <c r="B146" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C146" t="s">
         <v>4</v>
@@ -2425,7 +2767,7 @@
         <v>149</v>
       </c>
       <c r="B147" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C147" t="s">
         <v>4</v>
@@ -2436,7 +2778,7 @@
         <v>150</v>
       </c>
       <c r="B148" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C148" t="s">
         <v>4</v>
@@ -2447,7 +2789,7 @@
         <v>151</v>
       </c>
       <c r="B149" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C149" t="s">
         <v>4</v>
@@ -2458,7 +2800,7 @@
         <v>152</v>
       </c>
       <c r="B150" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C150" t="s">
         <v>4</v>
@@ -2469,7 +2811,7 @@
         <v>153</v>
       </c>
       <c r="B151" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C151" t="s">
         <v>4</v>
@@ -2480,7 +2822,7 @@
         <v>154</v>
       </c>
       <c r="B152" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C152" t="s">
         <v>4</v>
@@ -2491,7 +2833,7 @@
         <v>155</v>
       </c>
       <c r="B153" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C153" t="s">
         <v>4</v>
@@ -2502,9 +2844,1263 @@
         <v>156</v>
       </c>
       <c r="B154" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C154" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>157</v>
+      </c>
+      <c r="B155" t="n">
+        <v>13</v>
+      </c>
+      <c r="C155" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>158</v>
+      </c>
+      <c r="B156" t="n">
+        <v>13</v>
+      </c>
+      <c r="C156" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>159</v>
+      </c>
+      <c r="B157" t="n">
+        <v>10</v>
+      </c>
+      <c r="C157" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>160</v>
+      </c>
+      <c r="B158" t="n">
+        <v>10</v>
+      </c>
+      <c r="C158" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>161</v>
+      </c>
+      <c r="B159" t="n">
+        <v>10</v>
+      </c>
+      <c r="C159" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>162</v>
+      </c>
+      <c r="B160" t="n">
+        <v>7</v>
+      </c>
+      <c r="C160" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>163</v>
+      </c>
+      <c r="B161" t="n">
+        <v>7</v>
+      </c>
+      <c r="C161" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>164</v>
+      </c>
+      <c r="B162" t="n">
+        <v>6</v>
+      </c>
+      <c r="C162" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>165</v>
+      </c>
+      <c r="B163" t="n">
+        <v>6</v>
+      </c>
+      <c r="C163" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>166</v>
+      </c>
+      <c r="B164" t="n">
+        <v>6</v>
+      </c>
+      <c r="C164" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>167</v>
+      </c>
+      <c r="B165" t="n">
+        <v>6</v>
+      </c>
+      <c r="C165" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>168</v>
+      </c>
+      <c r="B166" t="n">
+        <v>6</v>
+      </c>
+      <c r="C166" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>169</v>
+      </c>
+      <c r="B167" t="n">
+        <v>6</v>
+      </c>
+      <c r="C167" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>170</v>
+      </c>
+      <c r="B168" t="n">
+        <v>6</v>
+      </c>
+      <c r="C168" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>171</v>
+      </c>
+      <c r="B169" t="n">
+        <v>6</v>
+      </c>
+      <c r="C169" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>172</v>
+      </c>
+      <c r="B170" t="n">
+        <v>6</v>
+      </c>
+      <c r="C170" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>173</v>
+      </c>
+      <c r="B171" t="n">
+        <v>4</v>
+      </c>
+      <c r="C171" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>174</v>
+      </c>
+      <c r="B172" t="n">
+        <v>4</v>
+      </c>
+      <c r="C172" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>175</v>
+      </c>
+      <c r="B173" t="n">
+        <v>4</v>
+      </c>
+      <c r="C173" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>176</v>
+      </c>
+      <c r="B174" t="n">
+        <v>4</v>
+      </c>
+      <c r="C174" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>177</v>
+      </c>
+      <c r="B175" t="n">
+        <v>4</v>
+      </c>
+      <c r="C175" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>178</v>
+      </c>
+      <c r="B176" t="n">
+        <v>4</v>
+      </c>
+      <c r="C176" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>179</v>
+      </c>
+      <c r="B177" t="n">
+        <v>4</v>
+      </c>
+      <c r="C177" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>180</v>
+      </c>
+      <c r="B178" t="n">
+        <v>4</v>
+      </c>
+      <c r="C178" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>181</v>
+      </c>
+      <c r="B179" t="n">
+        <v>4</v>
+      </c>
+      <c r="C179" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>182</v>
+      </c>
+      <c r="B180" t="n">
+        <v>4</v>
+      </c>
+      <c r="C180" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>183</v>
+      </c>
+      <c r="B181" t="n">
+        <v>4</v>
+      </c>
+      <c r="C181" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>184</v>
+      </c>
+      <c r="B182" t="n">
+        <v>4</v>
+      </c>
+      <c r="C182" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>185</v>
+      </c>
+      <c r="B183" t="n">
+        <v>4</v>
+      </c>
+      <c r="C183" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>186</v>
+      </c>
+      <c r="B184" t="n">
+        <v>3</v>
+      </c>
+      <c r="C184" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>187</v>
+      </c>
+      <c r="B185" t="n">
+        <v>3</v>
+      </c>
+      <c r="C185" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>188</v>
+      </c>
+      <c r="B186" t="n">
+        <v>3</v>
+      </c>
+      <c r="C186" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>189</v>
+      </c>
+      <c r="B187" t="n">
+        <v>3</v>
+      </c>
+      <c r="C187" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>190</v>
+      </c>
+      <c r="B188" t="n">
+        <v>3</v>
+      </c>
+      <c r="C188" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>191</v>
+      </c>
+      <c r="B189" t="n">
+        <v>3</v>
+      </c>
+      <c r="C189" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>192</v>
+      </c>
+      <c r="B190" t="n">
+        <v>3</v>
+      </c>
+      <c r="C190" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>193</v>
+      </c>
+      <c r="B191" t="n">
+        <v>3</v>
+      </c>
+      <c r="C191" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>194</v>
+      </c>
+      <c r="B192" t="n">
+        <v>3</v>
+      </c>
+      <c r="C192" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s">
+        <v>195</v>
+      </c>
+      <c r="B193" t="n">
+        <v>2</v>
+      </c>
+      <c r="C193" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>196</v>
+      </c>
+      <c r="B194" t="n">
+        <v>2</v>
+      </c>
+      <c r="C194" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s">
+        <v>197</v>
+      </c>
+      <c r="B195" t="n">
+        <v>2</v>
+      </c>
+      <c r="C195" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s">
+        <v>198</v>
+      </c>
+      <c r="B196" t="n">
+        <v>2</v>
+      </c>
+      <c r="C196" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s">
+        <v>199</v>
+      </c>
+      <c r="B197" t="n">
+        <v>2</v>
+      </c>
+      <c r="C197" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s">
+        <v>200</v>
+      </c>
+      <c r="B198" t="n">
+        <v>2</v>
+      </c>
+      <c r="C198" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>201</v>
+      </c>
+      <c r="B199" t="n">
+        <v>2</v>
+      </c>
+      <c r="C199" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>202</v>
+      </c>
+      <c r="B200" t="n">
+        <v>2</v>
+      </c>
+      <c r="C200" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s">
+        <v>203</v>
+      </c>
+      <c r="B201" t="n">
+        <v>2</v>
+      </c>
+      <c r="C201" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>204</v>
+      </c>
+      <c r="B202" t="n">
+        <v>2</v>
+      </c>
+      <c r="C202" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>205</v>
+      </c>
+      <c r="B203" t="n">
+        <v>2</v>
+      </c>
+      <c r="C203" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>206</v>
+      </c>
+      <c r="B204" t="n">
+        <v>2</v>
+      </c>
+      <c r="C204" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>207</v>
+      </c>
+      <c r="B205" t="n">
+        <v>2</v>
+      </c>
+      <c r="C205" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>208</v>
+      </c>
+      <c r="B206" t="n">
+        <v>2</v>
+      </c>
+      <c r="C206" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>209</v>
+      </c>
+      <c r="B207" t="n">
+        <v>2</v>
+      </c>
+      <c r="C207" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>210</v>
+      </c>
+      <c r="B208" t="n">
+        <v>2</v>
+      </c>
+      <c r="C208" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>211</v>
+      </c>
+      <c r="B209" t="n">
+        <v>2</v>
+      </c>
+      <c r="C209" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>212</v>
+      </c>
+      <c r="B210" t="n">
+        <v>2</v>
+      </c>
+      <c r="C210" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>213</v>
+      </c>
+      <c r="B211" t="n">
+        <v>2</v>
+      </c>
+      <c r="C211" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>214</v>
+      </c>
+      <c r="B212" t="n">
+        <v>2</v>
+      </c>
+      <c r="C212" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>215</v>
+      </c>
+      <c r="B213" t="n">
+        <v>2</v>
+      </c>
+      <c r="C213" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>216</v>
+      </c>
+      <c r="B214" t="n">
+        <v>2</v>
+      </c>
+      <c r="C214" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s">
+        <v>217</v>
+      </c>
+      <c r="B215" t="n">
+        <v>2</v>
+      </c>
+      <c r="C215" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s">
+        <v>218</v>
+      </c>
+      <c r="B216" t="n">
+        <v>2</v>
+      </c>
+      <c r="C216" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s">
+        <v>219</v>
+      </c>
+      <c r="B217" t="n">
+        <v>2</v>
+      </c>
+      <c r="C217" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s">
+        <v>220</v>
+      </c>
+      <c r="B218" t="n">
+        <v>2</v>
+      </c>
+      <c r="C218" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s">
+        <v>221</v>
+      </c>
+      <c r="B219" t="n">
+        <v>2</v>
+      </c>
+      <c r="C219" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s">
+        <v>222</v>
+      </c>
+      <c r="B220" t="n">
+        <v>1</v>
+      </c>
+      <c r="C220" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s">
+        <v>223</v>
+      </c>
+      <c r="B221" t="n">
+        <v>1</v>
+      </c>
+      <c r="C221" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s">
+        <v>224</v>
+      </c>
+      <c r="B222" t="n">
+        <v>1</v>
+      </c>
+      <c r="C222" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s">
+        <v>225</v>
+      </c>
+      <c r="B223" t="n">
+        <v>1</v>
+      </c>
+      <c r="C223" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s">
+        <v>226</v>
+      </c>
+      <c r="B224" t="n">
+        <v>1</v>
+      </c>
+      <c r="C224" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s">
+        <v>227</v>
+      </c>
+      <c r="B225" t="n">
+        <v>1</v>
+      </c>
+      <c r="C225" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s">
+        <v>228</v>
+      </c>
+      <c r="B226" t="n">
+        <v>1</v>
+      </c>
+      <c r="C226" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s">
+        <v>229</v>
+      </c>
+      <c r="B227" t="n">
+        <v>1</v>
+      </c>
+      <c r="C227" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s">
+        <v>230</v>
+      </c>
+      <c r="B228" t="n">
+        <v>1</v>
+      </c>
+      <c r="C228" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s">
+        <v>231</v>
+      </c>
+      <c r="B229" t="n">
+        <v>1</v>
+      </c>
+      <c r="C229" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s">
+        <v>232</v>
+      </c>
+      <c r="B230" t="n">
+        <v>1</v>
+      </c>
+      <c r="C230" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s">
+        <v>233</v>
+      </c>
+      <c r="B231" t="n">
+        <v>1</v>
+      </c>
+      <c r="C231" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s">
+        <v>234</v>
+      </c>
+      <c r="B232" t="n">
+        <v>1</v>
+      </c>
+      <c r="C232" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>235</v>
+      </c>
+      <c r="B233" t="n">
+        <v>1</v>
+      </c>
+      <c r="C233" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>236</v>
+      </c>
+      <c r="B234" t="n">
+        <v>1</v>
+      </c>
+      <c r="C234" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s">
+        <v>237</v>
+      </c>
+      <c r="B235" t="n">
+        <v>1</v>
+      </c>
+      <c r="C235" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s">
+        <v>238</v>
+      </c>
+      <c r="B236" t="n">
+        <v>1</v>
+      </c>
+      <c r="C236" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>239</v>
+      </c>
+      <c r="B237" t="n">
+        <v>1</v>
+      </c>
+      <c r="C237" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>240</v>
+      </c>
+      <c r="B238" t="n">
+        <v>1</v>
+      </c>
+      <c r="C238" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>241</v>
+      </c>
+      <c r="B239" t="n">
+        <v>1</v>
+      </c>
+      <c r="C239" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s">
+        <v>242</v>
+      </c>
+      <c r="B240" t="n">
+        <v>1</v>
+      </c>
+      <c r="C240" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s">
+        <v>243</v>
+      </c>
+      <c r="B241" t="n">
+        <v>1</v>
+      </c>
+      <c r="C241" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="s">
+        <v>244</v>
+      </c>
+      <c r="B242" t="n">
+        <v>1</v>
+      </c>
+      <c r="C242" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="s">
+        <v>245</v>
+      </c>
+      <c r="B243" t="n">
+        <v>1</v>
+      </c>
+      <c r="C243" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s">
+        <v>246</v>
+      </c>
+      <c r="B244" t="n">
+        <v>1</v>
+      </c>
+      <c r="C244" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s">
+        <v>247</v>
+      </c>
+      <c r="B245" t="n">
+        <v>1</v>
+      </c>
+      <c r="C245" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="s">
+        <v>248</v>
+      </c>
+      <c r="B246" t="n">
+        <v>1</v>
+      </c>
+      <c r="C246" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="s">
+        <v>249</v>
+      </c>
+      <c r="B247" t="n">
+        <v>1</v>
+      </c>
+      <c r="C247" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="s">
+        <v>250</v>
+      </c>
+      <c r="B248" t="n">
+        <v>1</v>
+      </c>
+      <c r="C248" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s">
+        <v>251</v>
+      </c>
+      <c r="B249" t="n">
+        <v>1</v>
+      </c>
+      <c r="C249" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="s">
+        <v>252</v>
+      </c>
+      <c r="B250" t="n">
+        <v>1</v>
+      </c>
+      <c r="C250" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="s">
+        <v>253</v>
+      </c>
+      <c r="B251" t="n">
+        <v>1</v>
+      </c>
+      <c r="C251" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s">
+        <v>254</v>
+      </c>
+      <c r="B252" t="n">
+        <v>1</v>
+      </c>
+      <c r="C252" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="s">
+        <v>255</v>
+      </c>
+      <c r="B253" t="n">
+        <v>1</v>
+      </c>
+      <c r="C253" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="s">
+        <v>256</v>
+      </c>
+      <c r="B254" t="n">
+        <v>1</v>
+      </c>
+      <c r="C254" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s">
+        <v>257</v>
+      </c>
+      <c r="B255" t="n">
+        <v>1</v>
+      </c>
+      <c r="C255" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s">
+        <v>258</v>
+      </c>
+      <c r="B256" t="n">
+        <v>1</v>
+      </c>
+      <c r="C256" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s">
+        <v>259</v>
+      </c>
+      <c r="B257" t="n">
+        <v>1</v>
+      </c>
+      <c r="C257" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s">
+        <v>260</v>
+      </c>
+      <c r="B258" t="n">
+        <v>1</v>
+      </c>
+      <c r="C258" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="s">
+        <v>261</v>
+      </c>
+      <c r="B259" t="n">
+        <v>1</v>
+      </c>
+      <c r="C259" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="s">
+        <v>262</v>
+      </c>
+      <c r="B260" t="n">
+        <v>1</v>
+      </c>
+      <c r="C260" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s">
+        <v>263</v>
+      </c>
+      <c r="B261" t="n">
+        <v>1</v>
+      </c>
+      <c r="C261" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="s">
+        <v>264</v>
+      </c>
+      <c r="B262" t="n">
+        <v>1</v>
+      </c>
+      <c r="C262" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="s">
+        <v>265</v>
+      </c>
+      <c r="B263" t="n">
+        <v>1</v>
+      </c>
+      <c r="C263" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="s">
+        <v>266</v>
+      </c>
+      <c r="B264" t="n">
+        <v>1</v>
+      </c>
+      <c r="C264" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="s">
+        <v>267</v>
+      </c>
+      <c r="B265" t="n">
+        <v>1</v>
+      </c>
+      <c r="C265" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>268</v>
+      </c>
+      <c r="B266" t="n">
+        <v>1</v>
+      </c>
+      <c r="C266" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="s">
+        <v>269</v>
+      </c>
+      <c r="B267" t="n">
+        <v>1</v>
+      </c>
+      <c r="C267" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s">
+        <v>270</v>
+      </c>
+      <c r="B268" t="n">
+        <v>1</v>
+      </c>
+      <c r="C268" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>